<commit_message>
fix data for continue integration
</commit_message>
<xml_diff>
--- a/src/main/resources/archetype-resources/src/test/resources/data/in/jouerAuJeuDesLogos.xlsx
+++ b/src/main/resources/archetype-resources/src/test/resources/data/in/jouerAuJeuDesLogos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="14670" windowHeight="5745"/>
@@ -37,15 +37,9 @@
     <t>amazon</t>
   </si>
   <si>
-    <t>burgerking</t>
-  </si>
-  <si>
     <t>ebay</t>
   </si>
   <si>
-    <t>hellokitty</t>
-  </si>
-  <si>
     <t>michelin</t>
   </si>
   <si>
@@ -83,12 +77,18 @@
   </si>
   <si>
     <t>heineken</t>
+  </si>
+  <si>
+    <t>burger king</t>
+  </si>
+  <si>
+    <t>hello kitty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -225,6 +225,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -272,7 +275,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -307,7 +310,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -518,9 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -538,7 +539,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -560,7 +561,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="6"/>
@@ -571,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="6"/>
@@ -582,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="5"/>
@@ -593,7 +594,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C6" s="7"/>
       <c r="E6" s="3"/>
@@ -603,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="6"/>
@@ -625,7 +626,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="6"/>
@@ -635,7 +636,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="5"/>
@@ -646,7 +647,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="6"/>
@@ -657,7 +658,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="6"/>
@@ -668,7 +669,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="5"/>
@@ -679,7 +680,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="6"/>
@@ -690,7 +691,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="6"/>
@@ -701,31 +702,31 @@
         <v>4</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>5</v>
@@ -738,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C20" s="7"/>
     </row>
@@ -747,7 +748,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C21" s="7"/>
     </row>
@@ -756,7 +757,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C22" s="7"/>
     </row>
@@ -765,7 +766,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C23" s="7"/>
     </row>
@@ -774,13 +775,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>5</v>
@@ -791,27 +792,27 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix data for continuous integration
</commit_message>
<xml_diff>
--- a/src/main/resources/archetype-resources/src/test/resources/data/in/jouerAuJeuDesLogos.xlsx
+++ b/src/main/resources/archetype-resources/src/test/resources/data/in/jouerAuJeuDesLogos.xlsx
@@ -49,9 +49,6 @@
     <t>pringles</t>
   </si>
   <si>
-    <t>redbull</t>
-  </si>
-  <si>
     <t>reebook</t>
   </si>
   <si>
@@ -83,6 +80,9 @@
   </si>
   <si>
     <t>hello kitty</t>
+  </si>
+  <si>
+    <t>red bull</t>
   </si>
 </sst>
 </file>
@@ -521,7 +521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -539,7 +541,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -561,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="6"/>
@@ -572,7 +574,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="6"/>
@@ -594,7 +596,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="7"/>
       <c r="E6" s="3"/>
@@ -626,7 +628,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="6"/>
@@ -658,7 +660,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="6"/>
@@ -680,7 +682,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="6"/>
@@ -708,25 +710,25 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>5</v>
@@ -748,7 +750,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C21" s="7"/>
     </row>
@@ -757,7 +759,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22" s="7"/>
     </row>
@@ -766,7 +768,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C23" s="7"/>
     </row>
@@ -775,13 +777,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>5</v>
@@ -792,7 +794,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>7</v>
@@ -800,19 +802,19 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>19</v>
       </c>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>